<commit_message>
Added Kurt's team coord
</commit_message>
<xml_diff>
--- a/Team-Coordination_team18_sec005.xlsx
+++ b/Team-Coordination_team18_sec005.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Documents\GitHub\engr132\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="25600" windowHeight="16080"/>
+    <workbookView xWindow="0" yWindow="-435" windowWidth="25605" windowHeight="16080"/>
   </bookViews>
   <sheets>
     <sheet name="Team18-April 22, 2014" sheetId="1" r:id="rId1"/>
@@ -24,7 +29,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="D9" authorId="0">
+    <comment ref="D9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0">
+    <comment ref="G9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0">
+    <comment ref="I9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="0">
+    <comment ref="K9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L9" authorId="0">
+    <comment ref="L9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A17" authorId="0">
+    <comment ref="A17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0">
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0">
+    <comment ref="F17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0">
+    <comment ref="I17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J17" authorId="0">
+    <comment ref="J17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -247,7 +252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A31" authorId="0">
+    <comment ref="A31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D31" authorId="0">
+    <comment ref="D31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -316,7 +321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E31" authorId="0">
+    <comment ref="E31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -344,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G31" authorId="0">
+    <comment ref="G31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -360,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I31" authorId="0">
+    <comment ref="I31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -390,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K31" authorId="0">
+    <comment ref="K31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C39" authorId="0">
+    <comment ref="C39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -421,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D39" authorId="0">
+    <comment ref="D39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -451,7 +456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E39" authorId="0">
+    <comment ref="E39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -568,7 +573,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F39" authorId="0">
+    <comment ref="F39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -595,7 +600,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G39" authorId="0">
+    <comment ref="G39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -611,7 +616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H39" authorId="0">
+    <comment ref="H39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -627,7 +632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J39" authorId="0">
+    <comment ref="J39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -659,7 +664,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
   <si>
     <t>Include a color to each row</t>
   </si>
@@ -922,44 +927,41 @@
     <t>Tsk10</t>
   </si>
   <si>
-    <t>Graph acc</t>
-  </si>
-  <si>
-    <t>Jake</t>
-  </si>
-  <si>
-    <t>4/10-4/29</t>
-  </si>
-  <si>
-    <t>4/10-2/29</t>
-  </si>
-  <si>
-    <t>Kurt</t>
-  </si>
-  <si>
-    <t>Evan</t>
-  </si>
-  <si>
-    <t>Make slider work</t>
-  </si>
-  <si>
-    <t>Allow radial buttons and slider to input to graph</t>
-  </si>
-  <si>
-    <t>Take input from slider and button</t>
-  </si>
-  <si>
-    <t>Allow input to graph</t>
-  </si>
-  <si>
-    <t>Nelson</t>
+    <t>Add names and headers to GUI</t>
+  </si>
+  <si>
+    <t>&lt; 1</t>
+  </si>
+  <si>
+    <t>Layouts must be finished for all guis</t>
+  </si>
+  <si>
+    <t>April 17 - April 18</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>The GUIs now have team member names on them as well as the project header at the beginning of the .m file.</t>
+  </si>
+  <si>
+    <t>All citations in APA format</t>
+  </si>
+  <si>
+    <t>Research should be done and pictures should be on GUI</t>
+  </si>
+  <si>
+    <t>Our citation page is in APA format and in-text citations are used.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1050,8 +1052,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1094,8 +1103,13 @@
         <bgColor rgb="FFDBEEF4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1204,42 +1218,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1265,14 +1288,64 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="TableStyleLight1" xfId="1" customBuiltin="1"/>
+    <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1344,908 +1417,19 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10073880" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="4762290" cy="9359720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="4762290" cy="9359720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="4762290" cy="9359720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="4762290" cy="9359720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="4762290" cy="9359720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="4762290" cy="9359720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -3419,232 +2603,47 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>666749</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>15875</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>15874</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Picture 25"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="shapetype_202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6000749" y="11366500"/>
-          <a:ext cx="2016125" cy="403225"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
       </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Picture 26"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6000750" y="12112625"/>
-          <a:ext cx="2000250" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>365126</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>587376</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>362542</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Picture 27"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5969000" y="11715751"/>
-          <a:ext cx="1952626" cy="378416"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="52" name="Picture 51"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6000750" y="10969625"/>
-          <a:ext cx="2016125" cy="403225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="53" name="Picture 52"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6000750" y="12493625"/>
-          <a:ext cx="2016125" cy="403225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="54" name="Picture 53"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6000750" y="12874625"/>
-          <a:ext cx="2016125" cy="403225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3972,907 +2971,963 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47:I47"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="17"/>
-      <c r="B2" s="13" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="18"/>
-      <c r="B3" s="13" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="19"/>
-      <c r="B4" s="13" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="20"/>
-      <c r="B5" s="13" t="s">
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="21"/>
-      <c r="B6" s="12" t="s">
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="8" spans="1:12" ht="21" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+    </row>
+    <row r="8" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1">
-      <c r="A9" s="10" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="s">
+      <c r="H9" s="20"/>
+      <c r="I9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="22" t="s">
+      <c r="J9" s="20"/>
+      <c r="K9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" customHeight="1">
-      <c r="A10" s="23" t="s">
+    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-    </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1">
-      <c r="A11" s="23" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-    </row>
-    <row r="12" spans="1:12" ht="30" customHeight="1">
-      <c r="A12" s="23" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-    </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1">
-      <c r="A13" s="23" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="I15" s="25"/>
-    </row>
-    <row r="16" spans="1:12" ht="21" customHeight="1">
-      <c r="A16" s="11" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-    </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1">
-      <c r="A17" s="10" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10" t="s">
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="22" t="s">
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-    </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1">
-      <c r="A18" s="7" t="s">
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+    </row>
+    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="27">
+      <c r="B18" s="22"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="14">
         <v>0</v>
       </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:12" ht="30" customHeight="1">
-      <c r="A19" s="5" t="s">
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="23"/>
+      <c r="C19" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="6" t="s">
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="27">
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="14">
         <v>0.5</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:12" ht="30" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+    </row>
+    <row r="20" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="6" t="s">
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="27">
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="14">
         <v>0.3</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="1:12" ht="30" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+    </row>
+    <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="23"/>
+      <c r="C21" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="6" t="s">
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="27">
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="14">
         <v>0.7</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="1:12" ht="30" customHeight="1">
-      <c r="A22" s="3" t="s">
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+    </row>
+    <row r="22" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="24"/>
+      <c r="C22" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="6" t="s">
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="27">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="14">
         <v>0.8</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="1:12" ht="30" customHeight="1">
-      <c r="A23" s="7" t="s">
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+    </row>
+    <row r="23" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="27">
+      <c r="B23" s="22"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="14">
         <v>0</v>
       </c>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="1:12" ht="30" customHeight="1">
-      <c r="A24" s="7" t="s">
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+    </row>
+    <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="27">
+      <c r="B24" s="22"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="14">
         <v>0</v>
       </c>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-    </row>
-    <row r="25" spans="1:12" ht="30" customHeight="1">
-      <c r="A25" s="5" t="s">
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+    </row>
+    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="8" t="s">
+      <c r="B25" s="23"/>
+      <c r="C25" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="6" t="s">
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="27">
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="14">
         <v>0.5</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-    </row>
-    <row r="26" spans="1:12" ht="30" customHeight="1">
-      <c r="A26" s="3" t="s">
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+    </row>
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="8" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="6" t="s">
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="27">
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="14">
         <v>0.8</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J26" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-    </row>
-    <row r="27" spans="1:12" ht="30" customHeight="1">
-      <c r="A27" s="7" t="s">
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+    </row>
+    <row r="27" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="6" t="s">
+      <c r="B27" s="22"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="27">
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="14">
         <v>0</v>
       </c>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-    </row>
-    <row r="30" spans="1:12" ht="21" customHeight="1">
-      <c r="A30" s="11" t="s">
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-    </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1">
-      <c r="A31" s="10" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+    </row>
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="22" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10" t="s">
+      <c r="F31" s="20"/>
+      <c r="G31" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10" t="s">
+      <c r="H31" s="20"/>
+      <c r="I31" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10" t="s">
+      <c r="J31" s="20"/>
+      <c r="K31" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="L31" s="10"/>
-    </row>
-    <row r="32" spans="1:12" ht="30" customHeight="1">
-      <c r="A32" s="23" t="s">
+      <c r="L31" s="20"/>
+    </row>
+    <row r="32" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="24" t="s">
+      <c r="C32" s="18"/>
+      <c r="D32" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="2" t="s">
+      <c r="F32" s="18"/>
+      <c r="G32" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="8" t="s">
+      <c r="H32" s="16"/>
+      <c r="I32" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-    </row>
-    <row r="33" spans="1:12" ht="30" customHeight="1">
-      <c r="A33" s="23" t="s">
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+    </row>
+    <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="24" t="s">
+      <c r="C33" s="18"/>
+      <c r="D33" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="2" t="s">
+      <c r="F33" s="18"/>
+      <c r="G33" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-    </row>
-    <row r="34" spans="1:12" ht="30" customHeight="1">
-      <c r="A34" s="23" t="s">
+      <c r="H33" s="16"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+    </row>
+    <row r="34" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-    </row>
-    <row r="35" spans="1:12" ht="30" customHeight="1">
-      <c r="A35" s="23" t="s">
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+    </row>
+    <row r="35" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-    </row>
-    <row r="38" spans="1:12" ht="21" customHeight="1">
-      <c r="A38" s="11" t="s">
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-    </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1">
-      <c r="A39" s="22" t="s">
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+    </row>
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D39" s="28" t="s">
+      <c r="D39" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E39" s="28" t="s">
+      <c r="E39" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F39" s="28" t="s">
+      <c r="F39" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="G39" s="28" t="s">
+      <c r="G39" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H39" s="10" t="s">
+      <c r="H39" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I39" s="10"/>
-      <c r="J39" s="1" t="s">
+      <c r="I39" s="20"/>
+      <c r="J39" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-    </row>
-    <row r="40" spans="1:12" ht="30" customHeight="1">
-      <c r="A40" s="23" t="s">
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+    </row>
+    <row r="40" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="24">
+      <c r="C40" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" s="31">
+        <v>1</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="G40" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="H40" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I40" s="32"/>
+      <c r="J40" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="K40" s="34"/>
+      <c r="L40" s="35"/>
+    </row>
+    <row r="41" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="31">
         <v>2</v>
       </c>
-      <c r="D40" s="24">
-        <v>8</v>
-      </c>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="G40" s="27">
-        <v>0.05</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-    </row>
-    <row r="41" spans="1:12" ht="30" customHeight="1">
-      <c r="A41" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="24">
-        <v>2</v>
-      </c>
-      <c r="D41" s="24">
-        <v>7</v>
-      </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="H41" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I41" s="32"/>
+      <c r="J41" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="K41" s="34"/>
+      <c r="L41" s="35"/>
+    </row>
+    <row r="42" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="F41" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="G41" s="27">
-        <v>0.05</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-    </row>
-    <row r="42" spans="1:12" ht="30" customHeight="1">
-      <c r="A42" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C42" s="24">
-        <v>2</v>
-      </c>
-      <c r="D42" s="24">
-        <v>8</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="G42" s="27">
-        <v>0.05</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-    </row>
-    <row r="43" spans="1:12" ht="30" customHeight="1">
-      <c r="A43" s="23" t="s">
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+    </row>
+    <row r="43" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="24">
-        <v>3</v>
-      </c>
-      <c r="D43" s="24">
-        <v>7</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="G43" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-    </row>
-    <row r="44" spans="1:12" ht="30" customHeight="1">
-      <c r="A44" s="23" t="s">
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+    </row>
+    <row r="44" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44" s="26">
-        <v>2</v>
-      </c>
-      <c r="D44" s="26">
-        <v>9</v>
-      </c>
-      <c r="E44" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="F44" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="G44" s="30">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I44" s="2"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-    </row>
-    <row r="45" spans="1:12" ht="30" customHeight="1">
-      <c r="A45" s="23" t="s">
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+    </row>
+    <row r="45" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="C45" s="26">
-        <v>2</v>
-      </c>
-      <c r="D45" s="26">
-        <v>7</v>
-      </c>
-      <c r="E45" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="F45" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="G45" s="30">
-        <v>0.1</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I45" s="2"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-    </row>
-    <row r="46" spans="1:12" ht="30" customHeight="1">
-      <c r="A46" s="23" t="s">
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+    </row>
+    <row r="46" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-    </row>
-    <row r="47" spans="1:12" ht="30" customHeight="1">
-      <c r="A47" s="23" t="s">
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+    </row>
+    <row r="47" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-    </row>
-    <row r="48" spans="1:12" ht="30" customHeight="1">
-      <c r="A48" s="23" t="s">
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+    </row>
+    <row r="48" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-    </row>
-    <row r="49" spans="1:12" ht="30" customHeight="1">
-      <c r="A49" s="23" t="s">
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+    </row>
+    <row r="49" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="120">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="A38:L38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:L42"/>
     <mergeCell ref="H48:I48"/>
     <mergeCell ref="J48:L48"/>
     <mergeCell ref="H49:I49"/>
@@ -4887,112 +3942,6 @@
     <mergeCell ref="J46:L46"/>
     <mergeCell ref="H47:I47"/>
     <mergeCell ref="J47:L47"/>
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" fitToHeight="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Switched names and worked out my part
</commit_message>
<xml_diff>
--- a/Team-Coordination_team18_sec005.xlsx
+++ b/Team-Coordination_team18_sec005.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ENGR132\GitHub\engr132\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Documents\GitHub\engr132\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -659,7 +659,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="139">
   <si>
     <t>Include a color to each row</t>
   </si>
@@ -679,9 +679,6 @@
     <t>Wow factor (only use for exceptional cases where element was exceptionally addressed)</t>
   </si>
   <si>
-    <t>Technical Coordinator -Jake Hallow</t>
-  </si>
-  <si>
     <t>Simulation Name</t>
   </si>
   <si>
@@ -763,9 +760,6 @@
     <t>Cohesive energy of nanoparticles</t>
   </si>
   <si>
-    <t>Design Coordinator -Nelson Luehrs</t>
-  </si>
-  <si>
     <t>Usability</t>
   </si>
   <si>
@@ -859,9 +853,6 @@
     <t>Not sure about this one, either</t>
   </si>
   <si>
-    <t>Evan Widloski – Educational Coordinator</t>
-  </si>
-  <si>
     <t>Learning Objective: The learner will be able to…</t>
   </si>
   <si>
@@ -955,9 +946,6 @@
     <t>How can the properties of increased bond strength be applied to everyday situations?</t>
   </si>
   <si>
-    <t>Team-Collaboration Coordinator -Kurt Sermersheim</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
@@ -1024,9 +1012,6 @@
     <t>Tsk6</t>
   </si>
   <si>
-    <t>Allow input to graph</t>
-  </si>
-  <si>
     <t>Nelson</t>
   </si>
   <si>
@@ -1045,18 +1030,6 @@
     <t>Next Round:</t>
   </si>
   <si>
-    <t>Jake Hallow - Design</t>
-  </si>
-  <si>
-    <t>Nelson Luehrs - Educational</t>
-  </si>
-  <si>
-    <t>Evan Widloski - Collaboration</t>
-  </si>
-  <si>
-    <t>Kurt Sermersheim - Technical</t>
-  </si>
-  <si>
     <t>Add names and header template to guis</t>
   </si>
   <si>
@@ -1067,13 +1040,49 @@
   </si>
   <si>
     <t>Evan, Jake, Kurt, and Nelson</t>
+  </si>
+  <si>
+    <t>Technical Coordinator -Kurt Sermersheim</t>
+  </si>
+  <si>
+    <t>Design Coordinator -Jake Hallow</t>
+  </si>
+  <si>
+    <t>Educational Coordinator - Evan Widloski</t>
+  </si>
+  <si>
+    <t>Team-Collaboration Coordinator -Nelson Luehrs</t>
+  </si>
+  <si>
+    <t>Jake Hallow - Education</t>
+  </si>
+  <si>
+    <t>Nelson Luehrs - Collaboration</t>
+  </si>
+  <si>
+    <t>Evan Widloski - Technical</t>
+  </si>
+  <si>
+    <t>Kurt Sermersheim - Design</t>
+  </si>
+  <si>
+    <t>Allow input be calculated</t>
+  </si>
+  <si>
+    <t>Develop Scenario more in-depth</t>
+  </si>
+  <si>
+    <t>4/24-present</t>
+  </si>
+  <si>
+    <t>Everybody</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1178,8 +1187,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1247,6 +1263,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -1360,46 +1381,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1434,20 +1425,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="12" borderId="8" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1470,12 +1449,8 @@
     <xf numFmtId="9" fontId="12" fillId="11" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="8" xfId="4" applyBorder="1"/>
     <xf numFmtId="9" fontId="13" fillId="12" borderId="8" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="8" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1485,10 +1460,77 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="8" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="9" xfId="5" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="9" xfId="5" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="9" xfId="5"/>
+    <xf numFmtId="9" fontId="14" fillId="13" borderId="9" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="9" xfId="5"/>
+    <xf numFmtId="9" fontId="14" fillId="13" borderId="9" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="9" xfId="5" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="10" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
@@ -2830,6 +2872,1110 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 46"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 44"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 42"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 40"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 38"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 36"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 34"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 32"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 30"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 28"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 26"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 24"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 22"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 20"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 18"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 16"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 14"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="AutoShape 12"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="AutoShape 10"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="AutoShape 8"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3101,8 +4247,8 @@
   </sheetPr>
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3115,1073 +4261,1084 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
     </row>
     <row r="8" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="A8" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="40"/>
+      <c r="I9" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="s">
+      <c r="J9" s="40"/>
+      <c r="K9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="22" t="s">
+      <c r="L9" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="C10" s="52"/>
+      <c r="D10" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53" t="s">
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="41" t="s">
+      <c r="L10" s="22" t="s">
         <v>16</v>
-      </c>
-      <c r="L10" s="41" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="C11" s="52"/>
+      <c r="D11" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53" t="s">
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="54" t="s">
+      <c r="H11" s="53"/>
+      <c r="I11" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54" t="s">
+      <c r="J11" s="53"/>
+      <c r="K11" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="J11" s="54"/>
-      <c r="K11" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="41" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="54" t="s">
+      <c r="H12" s="53"/>
+      <c r="I12" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54" t="s">
+      <c r="J12" s="53"/>
+      <c r="K12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="22" t="s">
         <v>27</v>
-      </c>
-      <c r="J12" s="54"/>
-      <c r="K12" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" s="41" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="C13" s="52"/>
+      <c r="D13" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53" t="s">
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="54" t="s">
+      <c r="H13" s="53"/>
+      <c r="I13" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="41" t="s">
-        <v>23</v>
+      <c r="J13" s="53"/>
+      <c r="K13" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="I15" s="24"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="A16" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10" t="s">
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10" t="s">
+      <c r="J17" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="26">
+      <c r="A18" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="13">
         <v>0</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="49"/>
+      <c r="C19" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="9" t="s">
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="J19" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="51"/>
+      <c r="C20" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="9" t="s">
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="J20" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="26">
-        <v>0.3</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="49"/>
+      <c r="C21" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="26">
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="13">
         <v>0.7</v>
       </c>
-      <c r="J21" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
+      <c r="J21" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="50"/>
+      <c r="C22" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="9" t="s">
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="J22" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="26">
-        <v>0.8</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="26">
+      <c r="A23" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="47"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="13">
         <v>0</v>
       </c>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="26">
+      <c r="A24" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="47"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="13">
         <v>0</v>
       </c>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="49"/>
+      <c r="C25" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="26">
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="13">
         <v>0.5</v>
       </c>
-      <c r="J25" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
+      <c r="J25" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="50"/>
+      <c r="C26" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="26">
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="13">
         <v>0.8</v>
       </c>
-      <c r="J26" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
+      <c r="J26" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="26">
+      <c r="A27" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="47"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="13">
         <v>0</v>
       </c>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
     </row>
     <row r="30" spans="1:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
+      <c r="A30" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
     </row>
     <row r="31" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="22" t="s">
+      <c r="H31" s="40"/>
+      <c r="I31" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="J31" s="40"/>
+      <c r="K31" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="L31" s="10"/>
+      <c r="L31" s="40"/>
     </row>
     <row r="32" spans="1:12" ht="71.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="45"/>
+      <c r="D32" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="F32" s="45"/>
+      <c r="G32" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="28" t="s">
+      <c r="H32" s="46"/>
+      <c r="I32" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="J32" s="45"/>
+      <c r="K32" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="L32" s="3"/>
+      <c r="L32" s="45"/>
     </row>
     <row r="33" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="43"/>
+      <c r="D33" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="F33" s="43"/>
+      <c r="G33" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="30" t="s">
+      <c r="H33" s="44"/>
+      <c r="I33" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H33" s="32"/>
-      <c r="I33" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
     </row>
     <row r="34" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="43"/>
+      <c r="D34" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="F34" s="43"/>
+      <c r="G34" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="30" t="s">
+      <c r="H34" s="44"/>
+      <c r="I34" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="H34" s="32"/>
-      <c r="I34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="43"/>
     </row>
     <row r="35" spans="1:12" ht="71.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="45"/>
+      <c r="D35" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="F35" s="45"/>
+      <c r="G35" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="28" t="s">
+      <c r="H35" s="46"/>
+      <c r="I35" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
+      <c r="A38" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="F39" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="G39" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="D39" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="F39" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="G39" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="I39" s="10"/>
-      <c r="J39" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="K39" s="33"/>
-      <c r="L39" s="33"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="K39" s="41"/>
+      <c r="L39" s="41"/>
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B40" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" s="37">
+      <c r="A40" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="57">
         <v>2</v>
       </c>
-      <c r="D40" s="37">
+      <c r="D40" s="57">
         <v>8</v>
       </c>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="G40" s="38">
-        <v>0.05</v>
-      </c>
-      <c r="H40" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="G40" s="61">
+        <v>0.2</v>
+      </c>
+      <c r="H40" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="62"/>
     </row>
     <row r="41" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="B41" s="45" t="s">
+      <c r="A41" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="27">
+        <v>2</v>
+      </c>
+      <c r="D41" s="27">
+        <v>7</v>
+      </c>
+      <c r="E41" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="46">
-        <v>2</v>
-      </c>
-      <c r="D41" s="46">
-        <v>7</v>
-      </c>
-      <c r="E41" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="F41" s="46" t="s">
-        <v>112</v>
-      </c>
-      <c r="G41" s="47">
-        <v>0.05</v>
-      </c>
-      <c r="H41" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
-      <c r="K41" s="48"/>
-      <c r="L41" s="48"/>
+      <c r="F41" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="H41" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
+      <c r="K41" s="42"/>
+      <c r="L41" s="42"/>
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="B42" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="C42" s="46">
+      <c r="A42" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="33">
         <v>2</v>
       </c>
-      <c r="D42" s="46">
+      <c r="D42" s="33">
         <v>8</v>
       </c>
-      <c r="E42" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="F42" s="46" t="s">
-        <v>108</v>
-      </c>
-      <c r="G42" s="47">
-        <v>0.05</v>
-      </c>
-      <c r="H42" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
-      <c r="K42" s="48"/>
-      <c r="L42" s="48"/>
+      <c r="E42" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="G42" s="63">
+        <v>1</v>
+      </c>
+      <c r="H42" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
     </row>
     <row r="43" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="B43" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="C43" s="37">
+      <c r="A43" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="57">
         <v>3</v>
       </c>
-      <c r="D43" s="37">
+      <c r="D43" s="57">
         <v>7</v>
       </c>
-      <c r="E43" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="F43" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="G43" s="38">
-        <v>0.1</v>
-      </c>
-      <c r="H43" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
+      <c r="E43" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="F43" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="G43" s="61">
+        <v>0.35</v>
+      </c>
+      <c r="H43" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="62"/>
     </row>
     <row r="44" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="B44" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="C44" s="49">
+      <c r="A44" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="29">
         <v>2</v>
       </c>
-      <c r="D44" s="49">
+      <c r="D44" s="29">
         <v>9</v>
       </c>
-      <c r="E44" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="F44" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="G44" s="50">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="H44" s="51" t="s">
-        <v>117</v>
-      </c>
-      <c r="I44" s="51"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
+      <c r="E44" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="G44" s="30">
+        <v>0.75</v>
+      </c>
+      <c r="H44" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
     </row>
     <row r="45" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="C45" s="42">
+      <c r="A45" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B45" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="25">
         <v>2</v>
       </c>
-      <c r="D45" s="42">
+      <c r="D45" s="25">
         <v>7</v>
       </c>
-      <c r="E45" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="F45" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="G45" s="43">
-        <v>0.1</v>
-      </c>
-      <c r="H45" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="44"/>
+      <c r="E45" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G45" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="H45" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="I45" s="38"/>
+      <c r="J45" s="38"/>
+      <c r="K45" s="38"/>
+      <c r="L45" s="38"/>
     </row>
     <row r="46" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="40" t="s">
+      <c r="A46" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="B46" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="C46" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="D46" s="42">
+      <c r="C46" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="23">
         <v>6</v>
       </c>
-      <c r="E46" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="G46" s="43">
-        <v>0.75</v>
-      </c>
-      <c r="H46" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
-      <c r="K46" s="44"/>
-      <c r="L46" s="44"/>
+      <c r="E46" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="G46" s="24">
+        <v>1</v>
+      </c>
+      <c r="H46" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
+      <c r="K46" s="38"/>
+      <c r="L46" s="38"/>
     </row>
     <row r="47" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
+      <c r="A47" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" s="58">
+        <v>1.5</v>
+      </c>
+      <c r="D47" s="58">
+        <v>5</v>
+      </c>
+      <c r="E47" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="G47" s="59">
+        <v>0.3</v>
+      </c>
+      <c r="H47" s="60" t="s">
+        <v>138</v>
+      </c>
+      <c r="I47" s="60"/>
+      <c r="J47" s="60"/>
+      <c r="K47" s="60"/>
+      <c r="L47" s="60"/>
     </row>
     <row r="48" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
+      <c r="A48" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
       <c r="H48" s="34"/>
       <c r="I48" s="34"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="35"/>
     </row>
     <row r="49" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
+      <c r="A49" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
       <c r="H49" s="34"/>
       <c r="I49" s="34"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
+      <c r="B52" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="36"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
+      <c r="B53" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" s="36"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B54" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
+      <c r="B54" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B55" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
+      <c r="B55" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B56" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="35"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
+      <c r="B56" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="125">
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="J48:L48"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:L49"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:L47"/>
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="J23:L23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="F24:H24"/>
@@ -4194,61 +5351,64 @@
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="F26:H26"/>
     <mergeCell ref="J26:L26"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="A38:L38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="J48:L48"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:L49"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>